<commit_message>
Izmena u kodu za stampanje - printFaker.
</commit_message>
<xml_diff>
--- a/domaci22.xlsx
+++ b/domaci22.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="156">
   <si>
     <t>Milan</t>
   </si>
@@ -97,6 +97,402 @@
   </si>
   <si>
     <t>Hammes</t>
+  </si>
+  <si>
+    <t>Audra</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>Corwin</t>
+  </si>
+  <si>
+    <t>Julieta</t>
+  </si>
+  <si>
+    <t>Howe</t>
+  </si>
+  <si>
+    <t>Garfield</t>
+  </si>
+  <si>
+    <t>Kerluke</t>
+  </si>
+  <si>
+    <t>Markus</t>
+  </si>
+  <si>
+    <t>Bauch</t>
+  </si>
+  <si>
+    <t>Craig</t>
+  </si>
+  <si>
+    <t>Pollich</t>
+  </si>
+  <si>
+    <t>Rob</t>
+  </si>
+  <si>
+    <t>Macejkovic</t>
+  </si>
+  <si>
+    <t>Debra</t>
+  </si>
+  <si>
+    <t>Osinski</t>
+  </si>
+  <si>
+    <t>Chet</t>
+  </si>
+  <si>
+    <t>Orn</t>
+  </si>
+  <si>
+    <t>Buster</t>
+  </si>
+  <si>
+    <t>Crona</t>
+  </si>
+  <si>
+    <t>Joaquin</t>
+  </si>
+  <si>
+    <t>Dooley</t>
+  </si>
+  <si>
+    <t>Gale</t>
+  </si>
+  <si>
+    <t>Becker</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>Brakus</t>
+  </si>
+  <si>
+    <t>Mardell</t>
+  </si>
+  <si>
+    <t>Bernhard</t>
+  </si>
+  <si>
+    <t>Gerard</t>
+  </si>
+  <si>
+    <t>Kunze</t>
+  </si>
+  <si>
+    <t>Yong</t>
+  </si>
+  <si>
+    <t>Harvey</t>
+  </si>
+  <si>
+    <t>Cinthia</t>
+  </si>
+  <si>
+    <t>Beer</t>
+  </si>
+  <si>
+    <t>Josephina</t>
+  </si>
+  <si>
+    <t>Gorczany</t>
+  </si>
+  <si>
+    <t>Daryl</t>
+  </si>
+  <si>
+    <t>Hansen</t>
+  </si>
+  <si>
+    <t>Errol</t>
+  </si>
+  <si>
+    <t>Marybelle</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Connie</t>
+  </si>
+  <si>
+    <t>Turner</t>
+  </si>
+  <si>
+    <t>Kieth</t>
+  </si>
+  <si>
+    <t>Konopelski</t>
+  </si>
+  <si>
+    <t>Lavonna</t>
+  </si>
+  <si>
+    <t>Gutkowski</t>
+  </si>
+  <si>
+    <t>Erasmo</t>
+  </si>
+  <si>
+    <t>Haag</t>
+  </si>
+  <si>
+    <t>Vernetta</t>
+  </si>
+  <si>
+    <t>Hessel</t>
+  </si>
+  <si>
+    <t>Leatha</t>
+  </si>
+  <si>
+    <t>Hauck</t>
+  </si>
+  <si>
+    <t>Rod</t>
+  </si>
+  <si>
+    <t>Pfannerstill</t>
+  </si>
+  <si>
+    <t>Jeff</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Wesley</t>
+  </si>
+  <si>
+    <t>Koss</t>
+  </si>
+  <si>
+    <t>Erin</t>
+  </si>
+  <si>
+    <t>Gusikowski</t>
+  </si>
+  <si>
+    <t>Marita</t>
+  </si>
+  <si>
+    <t>Dare</t>
+  </si>
+  <si>
+    <t>Carroll</t>
+  </si>
+  <si>
+    <t>Bins</t>
+  </si>
+  <si>
+    <t>Dorinda</t>
+  </si>
+  <si>
+    <t>Marvin</t>
+  </si>
+  <si>
+    <t>Batz</t>
+  </si>
+  <si>
+    <t>Dwain</t>
+  </si>
+  <si>
+    <t>Moen</t>
+  </si>
+  <si>
+    <t>Quiana</t>
+  </si>
+  <si>
+    <t>Rowe</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Hilde</t>
+  </si>
+  <si>
+    <t>Morar</t>
+  </si>
+  <si>
+    <t>Pierre</t>
+  </si>
+  <si>
+    <t>Kurtis</t>
+  </si>
+  <si>
+    <t>Pacocha</t>
+  </si>
+  <si>
+    <t>Danielle</t>
+  </si>
+  <si>
+    <t>Bahringer</t>
+  </si>
+  <si>
+    <t>Lupe</t>
+  </si>
+  <si>
+    <t>Mraz</t>
+  </si>
+  <si>
+    <t>Armand</t>
+  </si>
+  <si>
+    <t>Collier</t>
+  </si>
+  <si>
+    <t>Reynaldo</t>
+  </si>
+  <si>
+    <t>Berge</t>
+  </si>
+  <si>
+    <t>Marc</t>
+  </si>
+  <si>
+    <t>Kertzmann</t>
+  </si>
+  <si>
+    <t>Blossom</t>
+  </si>
+  <si>
+    <t>Priscilla</t>
+  </si>
+  <si>
+    <t>Goldner</t>
+  </si>
+  <si>
+    <t>Fredericka</t>
+  </si>
+  <si>
+    <t>Jeanie</t>
+  </si>
+  <si>
+    <t>Kovacek</t>
+  </si>
+  <si>
+    <t>Kaye</t>
+  </si>
+  <si>
+    <t>Bartoletti</t>
+  </si>
+  <si>
+    <t>Calvin</t>
+  </si>
+  <si>
+    <t>Kenyatta</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t>Verla</t>
+  </si>
+  <si>
+    <t>Windler</t>
+  </si>
+  <si>
+    <t>Lon</t>
+  </si>
+  <si>
+    <t>Barton</t>
+  </si>
+  <si>
+    <t>Alica</t>
+  </si>
+  <si>
+    <t>Kuvalis</t>
+  </si>
+  <si>
+    <t>Normand</t>
+  </si>
+  <si>
+    <t>Runte</t>
+  </si>
+  <si>
+    <t>Setsuko</t>
+  </si>
+  <si>
+    <t>Stehr</t>
+  </si>
+  <si>
+    <t>Traci</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Schneider</t>
+  </si>
+  <si>
+    <t>Mikel</t>
+  </si>
+  <si>
+    <t>Ullrich</t>
+  </si>
+  <si>
+    <t>Karen</t>
+  </si>
+  <si>
+    <t>Trantow</t>
+  </si>
+  <si>
+    <t>Hank</t>
+  </si>
+  <si>
+    <t>Jacobi</t>
+  </si>
+  <si>
+    <t>Pauletta</t>
+  </si>
+  <si>
+    <t>Jeremiah</t>
+  </si>
+  <si>
+    <t>Roberts</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Kassandra</t>
+  </si>
+  <si>
+    <t>Lebsack</t>
+  </si>
+  <si>
+    <t>Isreal</t>
+  </si>
+  <si>
+    <t>Hamill</t>
+  </si>
+  <si>
+    <t>Johnathon</t>
+  </si>
+  <si>
+    <t>Treutel</t>
+  </si>
+  <si>
+    <t>Rudy</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>Breitenberg</t>
+  </si>
+  <si>
+    <t>Hai</t>
   </si>
 </sst>
 </file>
@@ -455,15 +851,15 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>8</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>9</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>10</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>11</v>
@@ -471,50 +867,50 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>12</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>13</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>14</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>15</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>17</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>18</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>19</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>21</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>22</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Izmena u kodu za stampanje i dodati komentari kako rade metode.
</commit_message>
<xml_diff>
--- a/domaci22.xlsx
+++ b/domaci22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milla\IdeaProjects\Domaci2009\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422A4B5B-5D4E-4BD8-BF55-D408E31CEDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2627BF41-8C3E-4825-A1F0-B924CCFB3420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4230" yWindow="2025" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,20 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Milan</t>
-  </si>
-  <si>
-    <t>Stanojevic</t>
-  </si>
-  <si>
-    <t>Milos</t>
-  </si>
-  <si>
-    <t>Garunovic</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,31 +341,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B10"/>
+      <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>